<commit_message>
update metadata & rebasing input files
</commit_message>
<xml_diff>
--- a/data processing/Input Files/Metadata_File.xlsx
+++ b/data processing/Input Files/Metadata_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcrook\Documents\scenario_dashboard\data processing\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8B6B57-0133-4965-AB36-994749280987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B78F240A-64BD-4E35-900C-6C17F399DD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB5C35A7-A286-45A6-BD34-CA3CE6527B56}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB5C35A7-A286-45A6-BD34-CA3CE6527B56}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,9 +236,6 @@
     <t>Index (FY12=100)</t>
   </si>
   <si>
-    <t xml:space="preserve">Millions: 2019-20 prices </t>
-  </si>
-  <si>
     <t>CPAD</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>NATTOT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Millions: 2020-21 prices </t>
   </si>
 </sst>
 </file>
@@ -648,7 +648,7 @@
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D7" sqref="D7:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,10 +688,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>8</v>
@@ -700,10 +700,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -712,10 +712,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -724,10 +724,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>8</v>
@@ -745,7 +745,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -759,7 +759,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -773,7 +773,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -801,7 +801,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -843,7 +843,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -857,7 +857,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -885,7 +885,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -913,7 +913,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -941,7 +941,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -955,7 +955,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -969,7 +969,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -983,7 +983,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -997,7 +997,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1011,7 +1011,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1025,7 +1025,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -1044,7 +1044,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -1063,7 +1063,7 @@
         <v>9</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -1082,7 +1082,7 @@
         <v>9</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -1095,13 +1095,13 @@
         <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -1113,13 +1113,13 @@
         <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="I32" s="3"/>
       <c r="L32" s="3"/>
@@ -1135,7 +1135,7 @@
         <v>9</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1149,7 +1149,7 @@
         <v>9</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1176,30 +1176,30 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>